<commit_message>
MVC UPDDATE DetAIL POST
</commit_message>
<xml_diff>
--- a/temp_doc/KEGIATAN BKK.xlsx
+++ b/temp_doc/KEGIATAN BKK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/bkk/temp_doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9385EA9C-ADD4-3C45-B67F-BDC575C6913C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50E22B2-BCD7-1842-8FC9-702F7B160EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16480" xr2:uid="{70C81523-F9CB-7044-91B0-681474C867D0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>id_kegiatan_gambar</t>
   </si>
@@ -47,22 +47,49 @@
     <t>gambar</t>
   </si>
   <si>
-    <t>http://drive.google.com/uc?export=view&amp;id=13w5X3DADux2eT6wC0_r0Qveh2CQwBQWO</t>
-  </si>
-  <si>
-    <t>http://drive.google.com/uc?export=view&amp;id=142Hq3VVriJmJpMGwaBDJJMtc0tIPoa1N</t>
-  </si>
-  <si>
-    <t>http://drive.google.com/uc?export=view&amp;id=1RzmK3E6xZFPR2WQ3rvZL7shWMIAQKUnj</t>
-  </si>
-  <si>
-    <t>http://drive.google.com/uc?export=view&amp;id=1dUXTlBaloorrSGq_QwXZRhA9cAnQ7Iw4</t>
-  </si>
-  <si>
-    <t>http://drive.google.com/uc?export=view&amp;id=1h6_lBNVgXIzrvQRlDJbTlcxB2iaLrSab</t>
-  </si>
-  <si>
-    <t>http://drive.google.com/uc?export=view&amp;id=1vw4bTT15LoE4EHqr3eQjfMmEkoR8C7cH</t>
+    <t>http://drive.google.com/uc?export=view&amp;id=1OgocY18GorPFmFv0eLDahUkUYMlUfpT1</t>
+  </si>
+  <si>
+    <t>http://drive.google.com/uc?export=view&amp;id=1zUNOQxmQaiRCGZ6lcffwJXXFKqZk57gX</t>
+  </si>
+  <si>
+    <t>http://drive.google.com/uc?export=view&amp;id=1FwvvT4rbtmAPczGsuTpWqIOxmut2x2Z8</t>
+  </si>
+  <si>
+    <t>http://drive.google.com/uc?export=view&amp;id=18F6ZrsdrhkrmS5qdedS1-was6JY_rIK7</t>
+  </si>
+  <si>
+    <t>http://drive.google.com/uc?export=view&amp;id=1Gt33V9c8PukZh35uzJVIlZc9HzvE-qfZ</t>
+  </si>
+  <si>
+    <t>http://drive.google.com/uc?export=view&amp;id=1XwOryjrVcBVcyV0VtJHgskZ1MdPwubGB</t>
+  </si>
+  <si>
+    <t>http://drive.google.com/uc?export=view&amp;id=10J_GJrYmYl7IJ2G0aGCYdngSy94riw14</t>
+  </si>
+  <si>
+    <t>http://drive.google.com/uc?export=view&amp;id=1oZ6OI4S6aTHrhQXqZBh6lm7DIGoSSIjL</t>
+  </si>
+  <si>
+    <t>http://drive.google.com/uc?export=view&amp;id=1xij8W_3LBBMjfgmiJajkHniGuP2w_IzG</t>
+  </si>
+  <si>
+    <t>http://drive.google.com/uc?export=view&amp;id=1xWv8nrnCBfHXBORNuWR2qqoO5PwlP9bC</t>
+  </si>
+  <si>
+    <t>http://drive.google.com/uc?export=view&amp;id=1aqV8XnfHWUEYkgxqRuTPyYYk9vhkNT16</t>
+  </si>
+  <si>
+    <t>http://drive.google.com/uc?export=view&amp;id=1skHeJMFGoAITITsgDGFErVMZxRzPVBEw</t>
+  </si>
+  <si>
+    <t>http://drive.google.com/uc?export=view&amp;id=16zE4Ov7SwpOESg6whjsrtZ6wk0o_O8tx</t>
+  </si>
+  <si>
+    <t>http://drive.google.com/uc?export=view&amp;id=1PPBkCUQxRAHgDtn8WGjXKPxVgz3sjZPF</t>
+  </si>
+  <si>
+    <t>http://drive.google.com/uc?export=view&amp;id=1SyUli3s_yhkKsL7XyCoe0tJhG1xIesGG</t>
   </si>
 </sst>
 </file>
@@ -436,7 +463,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,10 +486,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1026</v>
+        <v>1036</v>
       </c>
       <c r="B2">
-        <v>2759</v>
+        <v>3617</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -470,10 +497,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1027</v>
+        <v>1037</v>
       </c>
       <c r="B3">
-        <v>2759</v>
+        <v>3617</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
@@ -481,10 +508,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1028</v>
+        <v>1038</v>
       </c>
       <c r="B4">
-        <v>2759</v>
+        <v>3617</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -492,10 +519,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1029</v>
+        <v>1039</v>
       </c>
       <c r="B5">
-        <v>2759</v>
+        <v>3617</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -503,10 +530,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1030</v>
+        <v>1040</v>
       </c>
       <c r="B6">
-        <v>2759</v>
+        <v>3617</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -514,41 +541,113 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1031</v>
+        <v>1041</v>
       </c>
       <c r="B7">
-        <v>2759</v>
+        <v>3617</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C8" s="2"/>
+      <c r="A8">
+        <v>1042</v>
+      </c>
+      <c r="B8">
+        <v>3617</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C9" s="2"/>
+      <c r="A9">
+        <v>1043</v>
+      </c>
+      <c r="B9">
+        <v>3617</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C10" s="2"/>
+      <c r="A10">
+        <v>1044</v>
+      </c>
+      <c r="B10">
+        <v>3617</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C11" s="2"/>
+      <c r="A11">
+        <v>1045</v>
+      </c>
+      <c r="B11">
+        <v>3617</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C12" s="2"/>
+      <c r="A12">
+        <v>1046</v>
+      </c>
+      <c r="B12">
+        <v>3617</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C13" s="2"/>
+      <c r="A13">
+        <v>1047</v>
+      </c>
+      <c r="B13">
+        <v>3617</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C14" s="2"/>
+      <c r="A14">
+        <v>1048</v>
+      </c>
+      <c r="B14">
+        <v>3617</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C15" s="2"/>
+      <c r="A15">
+        <v>1049</v>
+      </c>
+      <c r="B15">
+        <v>3617</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C16" s="2"/>
+      <c r="A16">
+        <v>1050</v>
+      </c>
+      <c r="B16">
+        <v>3617</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" s="2"/>
@@ -570,12 +669,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{6FA5AF7C-6382-1B4F-BB82-A7BF57F4EA50}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{31045BF2-8357-F346-829D-EEA47646D727}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{BFE5CA1A-19FA-8A47-9475-17C747A85615}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{F7352247-341B-0449-A7FB-EEFCB7CD209B}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{DDA7E8F9-4F8D-2C44-9AA5-200C92F82306}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{92C9D4E4-34CF-6C48-9C3E-73742F41182B}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{08F52978-9B10-6147-8550-5976ECA10206}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{0CFA5AF9-8927-334F-8527-EAC09EB71215}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{753A68E2-4B95-8C42-85CF-98D659BC1D23}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{26227327-7115-9A42-A792-30AAAE58DD13}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{31234FE3-5C82-CC4E-ABED-9932C117FAC1}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{31C9C211-7068-F64A-A92B-A3942F6AD2CE}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{D31D61BD-D1ED-9048-BFE0-57E47598A385}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00A4A718-E89E-EF48-90FC-C8013620FDD0}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{792F96C6-8A30-4E47-81C8-4A87777C7B8D}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{6E2E11BE-6C28-2D43-988C-4F0F92F5E43D}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{47DE9811-1948-AD40-97E9-3A475E49B634}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{D8840ED9-AC87-D44E-B71F-4C8BE94A82B6}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{A849641E-D6FE-8841-B439-055A42630DA9}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{4070199E-71AF-D24D-952C-E3C0DB7263A8}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{5E6309C6-91C9-8447-86FD-207BE69834D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>